<commit_message>
Changes done in MPT for Bangalore, Bhubaneswar, Noida and Pune-Mumbai
</commit_message>
<xml_diff>
--- a/Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack/Bhubaneswar/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_JDBC_MTT-Assessment.xlsx
+++ b/Bangalore_And_Bhubaneshwar (23rd_Sep) Batch_Java_Full_Stack/Bhubaneswar/MPT_MTT/Module 1/JavaFullStack-Module1_Java_SQL_JDBC_MTT-Assessment.xlsx
@@ -1325,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,10 +1335,10 @@
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="41.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="110" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="120.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>